<commit_message>
Chapter 1 and 6 changes
</commit_message>
<xml_diff>
--- a/Chapter 6 - The Middle - Publics/f6_4_uc_debt_income_time.xlsx
+++ b/Chapter 6 - The Middle - Publics/f6_4_uc_debt_income_time.xlsx
@@ -1,23 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Charlie/Dropbox/Stata_Notebooks/Bankers/chapter6/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Charlie/Dropbox/Stata_Notebooks/Bankers/Chapter 6 - The Middle - Publics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3333B6A8-12EC-2148-903C-6458015C4F5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E03C4C8-622F-D440-87A9-BBA81B292B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="460" windowWidth="27640" windowHeight="16940" xr2:uid="{A528BBA4-D868-2E42-A1DD-71B8130D0B1C}"/>
+    <workbookView xWindow="4780" yWindow="1980" windowWidth="23880" windowHeight="14180" xr2:uid="{A528BBA4-D868-2E42-A1DD-71B8130D0B1C}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <definedNames>
     <definedName name="hsgpadata">#REF!</definedName>
     <definedName name="transferdata">#REF!</definedName>
@@ -4199,35 +4196,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Chapter 2"/>
-      <sheetName val="2.1.1"/>
-      <sheetName val="2.1.2"/>
-      <sheetName val="2.2.1"/>
-      <sheetName val="2.2.2"/>
-      <sheetName val="2.3.1"/>
-      <sheetName val="2.3.2"/>
-      <sheetName val="2.3.4"/>
-      <sheetName val="2.3.5"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4528,7 +4496,7 @@
   <dimension ref="A1:L144"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>